<commit_message>
Added U8 part to BOM
</commit_message>
<xml_diff>
--- a/board/ekho_feb_bom.xlsx
+++ b/board/ekho_feb_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="155">
   <si>
     <t>Qty</t>
   </si>
@@ -475,13 +475,25 @@
   </si>
   <si>
     <t>2.5kΩ@100MHz</t>
+  </si>
+  <si>
+    <t>102-1319-ND</t>
+  </si>
+  <si>
+    <t>VAWQ6-Q24-D12H</t>
+  </si>
+  <si>
+    <t>CONV DC/DC DUAL 12V 230MA 6W</t>
+  </si>
+  <si>
+    <t>CUI Inc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -504,6 +516,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -549,12 +566,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -567,10 +587,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -902,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -911,7 +937,8 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="7" width="18" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="18" style="3" customWidth="1"/>
     <col min="9" max="9" width="34.5" customWidth="1"/>
     <col min="13" max="13" width="22.83203125" customWidth="1"/>
@@ -1727,26 +1754,36 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="6">
+      <c r="A27" s="8">
         <v>1</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
+      <c r="F27" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:M28">

</xml_diff>